<commit_message>
Atualizacao padronizacao css backlog
</commit_message>
<xml_diff>
--- a/TI/BACKLOG CLUB PENGUIN.xlsx
+++ b/TI/BACKLOG CLUB PENGUIN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isabela\Projeto-Individual\TI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isabela\Desktop\Projeto-Individual\TI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D666C013-4508-4C6E-8506-3B4F071D792A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F95CB5C-65E4-4953-BFD2-74175623A5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D5348C50-36D5-4FA6-A837-23633C402768}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D5348C50-36D5-4FA6-A837-23633C402768}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
   <si>
     <t>Backlog</t>
   </si>
@@ -181,6 +181,15 @@
   </si>
   <si>
     <t>Importante</t>
+  </si>
+  <si>
+    <t>Padronizar CSS</t>
+  </si>
+  <si>
+    <t>Padronização do CSS do site para facilitar a leitura do codigo</t>
+  </si>
+  <si>
+    <t>Desejavel</t>
   </si>
 </sst>
 </file>
@@ -602,22 +611,22 @@
   <dimension ref="D2:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.44140625" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.88671875" customWidth="1"/>
+    <col min="13" max="13" width="12.44140625" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D2" s="8" t="s">
         <v>0</v>
       </c>
@@ -627,7 +636,7 @@
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
@@ -656,7 +665,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="4:18" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:18" ht="86.4" x14ac:dyDescent="0.3">
       <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
@@ -681,7 +690,7 @@
       <c r="M4" s="7"/>
       <c r="N4" s="5"/>
     </row>
-    <row r="5" spans="4:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:18" ht="57.6" x14ac:dyDescent="0.3">
       <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
@@ -706,7 +715,7 @@
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
     </row>
-    <row r="6" spans="4:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D6" s="3" t="s">
         <v>14</v>
       </c>
@@ -729,7 +738,7 @@
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
     </row>
-    <row r="7" spans="4:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D7" s="2" t="s">
         <v>18</v>
       </c>
@@ -752,7 +761,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="4:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D8" s="3" t="s">
         <v>26</v>
       </c>
@@ -772,7 +781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="4:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
@@ -792,7 +801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="4:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D10" s="3" t="s">
         <v>25</v>
       </c>
@@ -812,7 +821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="4:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D11" s="2" t="s">
         <v>24</v>
       </c>
@@ -832,7 +841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="4:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D12" s="3" t="s">
         <v>27</v>
       </c>
@@ -852,7 +861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="4:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D13" s="2" t="s">
         <v>30</v>
       </c>
@@ -872,7 +881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="4:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D14" s="3" t="s">
         <v>31</v>
       </c>
@@ -892,7 +901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="4:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D15" s="2" t="s">
         <v>33</v>
       </c>
@@ -912,7 +921,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="4:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D16" s="3" t="s">
         <v>36</v>
       </c>
@@ -932,7 +941,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D17" s="2" t="s">
         <v>37</v>
       </c>
@@ -952,7 +961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="4:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D18" s="3" t="s">
         <v>44</v>
       </c>
@@ -972,7 +981,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="3">
+        <v>5</v>
+      </c>
+      <c r="I19" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -980,7 +1009,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -988,7 +1017,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -1005,15 +1034,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010003E766D4FE020D42BD39BDB2136774A4" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="06934da6e5b10321cb88d0fc1a3ce0fd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dc254948-99fa-45f6-a566-6a61bfbd02ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bcb8c8660b69ba97b99a21cf744ffae9" ns3:_="">
     <xsd:import namespace="dc254948-99fa-45f6-a566-6a61bfbd02ca"/>
@@ -1189,6 +1209,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1198,14 +1227,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2699B0C-C07C-4B7F-BF52-7219CED35FDB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FB5C2BC-BBD7-42DA-99CB-B2D0D5A450FC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1219,6 +1240,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2699B0C-C07C-4B7F-BF52-7219CED35FDB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Transferencia do HTML e CSS para o web-data-viz
</commit_message>
<xml_diff>
--- a/TI/BACKLOG CLUB PENGUIN.xlsx
+++ b/TI/BACKLOG CLUB PENGUIN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isabela\Desktop\Projeto-Individual\TI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F95CB5C-65E4-4953-BFD2-74175623A5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEE6005-FD08-4F20-9C1B-0AB33CC6BBA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D5348C50-36D5-4FA6-A837-23633C402768}"/>
+    <workbookView xWindow="2760" yWindow="2745" windowWidth="21600" windowHeight="11295" xr2:uid="{D5348C50-36D5-4FA6-A837-23633C402768}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
   <si>
     <t>Backlog</t>
   </si>
@@ -172,15 +172,6 @@
   </si>
   <si>
     <t>;</t>
-  </si>
-  <si>
-    <t>Prototipo do Site</t>
-  </si>
-  <si>
-    <t>Prototipo de todas as paginas do site na ferramenta figma</t>
-  </si>
-  <si>
-    <t>Importante</t>
   </si>
   <si>
     <t>Padronizar CSS</t>
@@ -608,25 +599,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F795EA-1BDC-4237-A8B0-3AA9F3C9EE38}">
-  <dimension ref="D2:R27"/>
+  <dimension ref="D2:R26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.44140625" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.88671875" customWidth="1"/>
-    <col min="13" max="13" width="12.44140625" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D2" s="8" t="s">
         <v>0</v>
       </c>
@@ -636,7 +627,7 @@
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
@@ -665,7 +656,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="4:18" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:18" ht="90" x14ac:dyDescent="0.25">
       <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
@@ -690,7 +681,7 @@
       <c r="M4" s="7"/>
       <c r="N4" s="5"/>
     </row>
-    <row r="5" spans="4:18" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:18" ht="60" x14ac:dyDescent="0.25">
       <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
@@ -709,13 +700,11 @@
       <c r="I5" s="2">
         <v>1</v>
       </c>
-      <c r="L5" s="6" t="s">
-        <v>43</v>
-      </c>
+      <c r="L5" s="6"/>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
     </row>
-    <row r="6" spans="4:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:18" ht="30" x14ac:dyDescent="0.25">
       <c r="D6" s="3" t="s">
         <v>14</v>
       </c>
@@ -738,7 +727,7 @@
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
     </row>
-    <row r="7" spans="4:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:18" ht="30" x14ac:dyDescent="0.25">
       <c r="D7" s="2" t="s">
         <v>18</v>
       </c>
@@ -761,7 +750,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="4:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:18" ht="30" x14ac:dyDescent="0.25">
       <c r="D8" s="3" t="s">
         <v>26</v>
       </c>
@@ -781,7 +770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="4:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:18" ht="30" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
@@ -801,7 +790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="4:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:18" ht="30" x14ac:dyDescent="0.25">
       <c r="D10" s="3" t="s">
         <v>25</v>
       </c>
@@ -821,7 +810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="4:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:18" ht="30" x14ac:dyDescent="0.25">
       <c r="D11" s="2" t="s">
         <v>24</v>
       </c>
@@ -841,7 +830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="4:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:18" ht="30" x14ac:dyDescent="0.25">
       <c r="D12" s="3" t="s">
         <v>27</v>
       </c>
@@ -861,7 +850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="4:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:18" ht="30" x14ac:dyDescent="0.25">
       <c r="D13" s="2" t="s">
         <v>30</v>
       </c>
@@ -881,7 +870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="4:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:18" ht="30" x14ac:dyDescent="0.25">
       <c r="D14" s="3" t="s">
         <v>31</v>
       </c>
@@ -901,7 +890,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="4:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:18" ht="30" x14ac:dyDescent="0.25">
       <c r="D15" s="2" t="s">
         <v>33</v>
       </c>
@@ -921,7 +910,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="4:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:18" ht="45" x14ac:dyDescent="0.25">
       <c r="D16" s="3" t="s">
         <v>36</v>
       </c>
@@ -941,7 +930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="4:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D17" s="2" t="s">
         <v>37</v>
       </c>
@@ -961,7 +950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="4:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D18" s="3" t="s">
         <v>44</v>
       </c>
@@ -972,36 +961,24 @@
         <v>46</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H18" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I18" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="4:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D19" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="3">
-        <v>5</v>
-      </c>
-      <c r="I19" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -1009,21 +986,13 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1034,6 +1003,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010003E766D4FE020D42BD39BDB2136774A4" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="06934da6e5b10321cb88d0fc1a3ce0fd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dc254948-99fa-45f6-a566-6a61bfbd02ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bcb8c8660b69ba97b99a21cf744ffae9" ns3:_="">
     <xsd:import namespace="dc254948-99fa-45f6-a566-6a61bfbd02ca"/>
@@ -1209,15 +1187,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1227,6 +1196,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2699B0C-C07C-4B7F-BF52-7219CED35FDB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FB5C2BC-BBD7-42DA-99CB-B2D0D5A450FC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1240,14 +1217,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2699B0C-C07C-4B7F-BF52-7219CED35FDB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>